<commit_message>
Added new options form
</commit_message>
<xml_diff>
--- a/TFSUtil/WindowsFormsApplication1/References/RTMTemplate.xlsx
+++ b/TFSUtil/WindowsFormsApplication1/References/RTMTemplate.xlsx
@@ -1400,56 +1400,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49eeb49d-9eb9-447f-a718-737c9def62db">
+      <Value>7</Value>
+      <Value>4</Value>
+      <Value>48</Value>
+    </TaxCatchAll>
+    <Reason_x0020_for_x0020_Exclusion xmlns="49eeb49d-9eb9-447f-a718-737c9def62db" xsi:nil="true"/>
+    <Searchable_x0020_in_x0020_KM xmlns="49eeb49d-9eb9-447f-a718-737c9def62db">Yes</Searchable_x0020_in_x0020_KM>
+    <_dlc_DocId xmlns="49eeb49d-9eb9-447f-a718-737c9def62db">CLDIV1-62-4102</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="49eeb49d-9eb9-447f-a718-737c9def62db">
+      <Url>http://icon.crimsonlogic.com/div1/oe/_layouts/DocIdRedir.aspx?ID=CLDIV1-62-4102</Url>
+      <Description>CLDIV1-62-4102</Description>
+    </_dlc_DocIdUrl>
+    <Created_x0020_By0 xmlns="1dd848b9-1366-4027-a7b1-f324a05e4b60" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B7DF73B6EAEFF141A4E8927527DC680A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14e034e687c0b4014f4f0af15f2a75f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1dd848b9-1366-4027-a7b1-f324a05e4b60" xmlns:ns3="49eeb49d-9eb9-447f-a718-737c9def62db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d5be2988f07e83462761569b2369c66" ns2:_="" ns3:_="">
     <xsd:import namespace="1dd848b9-1366-4027-a7b1-f324a05e4b60"/>
@@ -1636,24 +1606,54 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49eeb49d-9eb9-447f-a718-737c9def62db">
-      <Value>7</Value>
-      <Value>4</Value>
-      <Value>48</Value>
-    </TaxCatchAll>
-    <Reason_x0020_for_x0020_Exclusion xmlns="49eeb49d-9eb9-447f-a718-737c9def62db" xsi:nil="true"/>
-    <Searchable_x0020_in_x0020_KM xmlns="49eeb49d-9eb9-447f-a718-737c9def62db">Yes</Searchable_x0020_in_x0020_KM>
-    <_dlc_DocId xmlns="49eeb49d-9eb9-447f-a718-737c9def62db">CLDIV1-62-4102</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="49eeb49d-9eb9-447f-a718-737c9def62db">
-      <Url>http://icon.crimsonlogic.com/div1/oe/_layouts/DocIdRedir.aspx?ID=CLDIV1-62-4102</Url>
-      <Description>CLDIV1-62-4102</Description>
-    </_dlc_DocIdUrl>
-    <Created_x0020_By0 xmlns="1dd848b9-1366-4027-a7b1-f324a05e4b60" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1666,22 +1666,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9DCDA9C-BC82-44D4-834C-E437E1F148BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617EF815-9F09-4014-8480-1B986D19FC46}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="49eeb49d-9eb9-447f-a718-737c9def62db"/>
+    <ds:schemaRef ds:uri="1dd848b9-1366-4027-a7b1-f324a05e4b60"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AC7A54E-E7BA-4DA1-B990-4BCB85CB4D43}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB118FB9-8160-4E03-B131-0377557A0CD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1700,13 +1695,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AC7A54E-E7BA-4DA1-B990-4BCB85CB4D43}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617EF815-9F09-4014-8480-1B986D19FC46}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9DCDA9C-BC82-44D4-834C-E437E1F148BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="49eeb49d-9eb9-447f-a718-737c9def62db"/>
-    <ds:schemaRef ds:uri="1dd848b9-1366-4027-a7b1-f324a05e4b60"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>